<commit_message>
Upload Y2_B2526_Biochemistry_LAB_CBL_System_2025-10-05T12-14-09.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y2_B2526_Biochemistry_LAB_CBL_System_2025-10-05T12-14-09.xlsx
+++ b/log_history/Y2_B2526_Biochemistry_LAB_CBL_System_2025-10-05T12-14-09.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6207BB9B-1503-4C20-B384-E114167AC4C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD7BF4D-0B74-4CE5-81B4-157E913CA856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Biochemistry" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <t>System</t>
   </si>
   <si>
-    <t>Biochemistry LAB/CBL</t>
+    <t xml:space="preserve">Biochemistry Lab/CBL </t>
   </si>
 </sst>
 </file>

</xml_diff>